<commit_message>
moderate match only by strong adaption of boundaries to target range.
</commit_message>
<xml_diff>
--- a/Full_catalytic_performance_data_Zenodo_predict_vs_measure.xlsx
+++ b/Full_catalytic_performance_data_Zenodo_predict_vs_measure.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D38381-E513-433B-8CB0-29E1C6FBE432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE80D9C-A968-4D50-83DB-38304B5C6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5033,7 +5033,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH61" sqref="AH61"/>
+      <selection pane="bottomLeft" activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>

</xml_diff>